<commit_message>
update remove file XLSX
</commit_message>
<xml_diff>
--- a/src/excel/User.xlsx
+++ b/src/excel/User.xlsx
@@ -24,7 +24,98 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">realName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avtar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">createdAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updatedAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12112212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu Jun 16 2022 10:04:20 GMT+0700 (Indochina Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121as12212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu Jun 16 2022 10:04:25 GMT+0700 (Indochina Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">121212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed Jun 15 2022 15:49:19 GMT+0700 (Indochina Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri Jun 17 2022 08:53:10 GMT+0700 (Indochina Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ha Gia Dat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hihi@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hihihi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wed Jun 15 2022 15:15:13 GMT+0700 (Indochina Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri Jun 17 2022 08:53:51 GMT+0700 (Indochina Time)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -347,8 +438,135 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2"/>
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>